<commit_message>
update water quality parser
</commit_message>
<xml_diff>
--- a/bio_diversity/static/data_templates/coldbrook-water_quality_record.xlsx
+++ b/bio_diversity/static/data_templates/coldbrook-water_quality_record.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stoyelq\Desktop\Work\dm_apps\dm_apps\bio_diversity\static\data_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACFB6AAF-BB62-4C8D-98B4-AC3E40B3AA38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67115E7D-34D5-4CF6-8E55-A778E133E517}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="915" yWindow="960" windowWidth="24720" windowHeight="13680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Water Quality Data" sheetId="6" r:id="rId1"/>
@@ -45,9 +45,6 @@
     <t>Comments</t>
   </si>
   <si>
-    <t>Time (24HR)</t>
-  </si>
-  <si>
     <t>Dissolved Nitrogen %</t>
   </si>
   <si>
@@ -91,6 +88,9 @@
   </si>
   <si>
     <t>Optional. Eg. AB, CD</t>
+  </si>
+  <si>
+    <t>Time</t>
   </si>
 </sst>
 </file>
@@ -475,7 +475,7 @@
   <dimension ref="A2:L3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -490,16 +490,16 @@
   <sheetData>
     <row r="2" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="D2" s="1" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>0</v>
@@ -517,10 +517,10 @@
         <v>3</v>
       </c>
       <c r="J2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K2" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="L2" s="1" t="s">
         <v>5</v>
@@ -528,40 +528,40 @@
     </row>
     <row r="3" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="C3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="D3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="E3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="F3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="G3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="H3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="I3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="J3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="J3" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>21</v>
-      </c>
       <c r="L3" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>